<commit_message>
Finished queries and dashboard
</commit_message>
<xml_diff>
--- a/CovidTable3.xlsx
+++ b/CovidTable3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofutah-my.sharepoint.com/personal/u1156525_umail_utah_edu/Documents/Projects/Covid-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{69401028-EE23-4C76-9182-3011078A595E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B8F9DC2-E0DC-408F-896B-8D9D00725ED0}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{69401028-EE23-4C76-9182-3011078A595E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDC01AF7-E7C2-4D7A-89B5-83B7B77F45D3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6C13693-636D-43EC-95AF-BA83A6A2E8D5}"/>
   </bookViews>
@@ -1094,11 +1094,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18844A6C-67C3-4A14-AB98-A29CF72BE093}">
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>